<commit_message>
Updated example data set
</commit_message>
<xml_diff>
--- a/examples/simple/simple.xlsx
+++ b/examples/simple/simple.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kaklise\src\pecos\examples\simple\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,12 +93,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -574,37 +582,37 @@
                   <c:v>0.48958333321934333</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50004318117923363</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.5000883958138671</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50004872625137364</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50002930852966221</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50004590215260181</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50004156149239554</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50002453976568684</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50000382933616838</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50000658645567264</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50005799475611556</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.49999999988358468</c:v>
+                  <c:v>0.50003809867522442</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0.6145833331902395</c:v>
@@ -724,6 +732,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CCDD-4C66-8753-C5B676B65F69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1337,6 +1350,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CCDD-4C66-8753-C5B676B65F69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1950,6 +1968,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CCDD-4C66-8753-C5B676B65F69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2554,6 +2577,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CCDD-4C66-8753-C5B676B65F69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2876,6 +2904,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CCDD-4C66-8753-C5B676B65F69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2924,7 +2957,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3019,7 +3051,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3052,9 +3084,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3087,6 +3136,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3265,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49:H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4094,7 +4160,7 @@
         <v>42005.499999999884</v>
       </c>
       <c r="B49" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50004318117923363</v>
       </c>
       <c r="C49">
         <v>0.88327566536283564</v>
@@ -4111,7 +4177,7 @@
         <v>42005.510416666548</v>
       </c>
       <c r="B50" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.5000883958138671</v>
       </c>
       <c r="C50">
         <v>0.78683024839568083</v>
@@ -4128,7 +4194,7 @@
         <v>42005.520833333212</v>
       </c>
       <c r="B51" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50004872625137364</v>
       </c>
       <c r="C51">
         <v>0.42783700516933465</v>
@@ -4145,7 +4211,7 @@
         <v>42005.531249999876</v>
       </c>
       <c r="B52" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50002930852966221</v>
       </c>
       <c r="C52">
         <v>2.1097359198667509E-2</v>
@@ -4162,7 +4228,7 @@
         <v>42005.541666666541</v>
       </c>
       <c r="B53" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50004590215260181</v>
       </c>
       <c r="C53">
         <v>7.3028713324937877E-2</v>
@@ -4179,7 +4245,7 @@
         <v>42005.552083333205</v>
       </c>
       <c r="B54" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50004156149239554</v>
       </c>
       <c r="C54">
         <v>0.32839275681223123</v>
@@ -4196,7 +4262,7 @@
         <v>42005.562499999869</v>
       </c>
       <c r="B55" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50002453976568684</v>
       </c>
       <c r="C55">
         <v>0.37308792423602033</v>
@@ -4213,7 +4279,7 @@
         <v>42005.572916666533</v>
       </c>
       <c r="B56" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50000382933616838</v>
       </c>
       <c r="C56">
         <v>0.61879718750129209</v>
@@ -4230,7 +4296,7 @@
         <v>42005.583333333198</v>
       </c>
       <c r="B57" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50000658645567264</v>
       </c>
       <c r="C57">
         <v>0.57054023396486397</v>
@@ -4247,7 +4313,7 @@
         <v>42005.593749999862</v>
       </c>
       <c r="B58" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50005799475611556</v>
       </c>
       <c r="C58">
         <v>0.5650683952811788</v>
@@ -4264,7 +4330,7 @@
         <v>42005.604166666526</v>
       </c>
       <c r="B59" s="7">
-        <v>0.49999999988358468</v>
+        <v>0.50003809867522442</v>
       </c>
       <c r="C59">
         <v>0.98163360352978357</v>

</xml_diff>